<commit_message>
upload excel file validation
</commit_message>
<xml_diff>
--- a/storage/framework/laravel-excel/laravel-excel-bAmgdVd0NdEiqDsonT3XEL4dKcE0EiEF.xlsx
+++ b/storage/framework/laravel-excel/laravel-excel-bAmgdVd0NdEiqDsonT3XEL4dKcE0EiEF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive(hafizjamil265@gmail.com)\Project prim.my\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prim-development\storage\framework\laravel-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB51BC96-2B63-4DBA-9B74-B051E042E32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EAB01C-D822-4B94-B844-963C42845D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{11096705-C16A-4A4D-BF9D-0032818E2482}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{11096705-C16A-4A4D-BF9D-0032818E2482}"/>
   </bookViews>
   <sheets>
     <sheet name="5 AWAM 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="236">
   <si>
     <t>Bil</t>
   </si>
@@ -690,9 +690,6 @@
     <t>sharkawi2004@gmail.com</t>
   </si>
   <si>
-    <t>zikram1612gmail.com</t>
-  </si>
-  <si>
     <t>anisnabilah354@gmail.com</t>
   </si>
   <si>
@@ -744,7 +741,7 @@
     <t>Column1</t>
   </si>
   <si>
-    <t>Column14</t>
+    <t>zikram@1612gmail.com</t>
   </si>
 </sst>
 </file>
@@ -939,7 +936,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -964,6 +960,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1259,13 +1256,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1287,6 +1277,13 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1320,7 +1317,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFCE145A-C660-4D9D-B229-74C79ACBF807}" name="Table1" displayName="Table1" ref="A1:M30" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFCE145A-C660-4D9D-B229-74C79ACBF807}" name="Table1" displayName="Table1" ref="A1:M30" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M30" xr:uid="{DFCE145A-C660-4D9D-B229-74C79ACBF807}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{D68AA35B-0646-41D3-9998-D3E03CC50AAF}" name="Bil" dataDxfId="12"/>
@@ -1334,10 +1331,10 @@
     <tableColumn id="9" xr3:uid="{0424D710-A033-46FE-AFCE-97820E9A9E7A}" name="Nama Penjaga 2" dataDxfId="4"/>
     <tableColumn id="10" xr3:uid="{752AB41B-C136-4C6C-B35A-CE4B43F63C30}" name="No. Tel Bimbit Penjaga 2" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{5B74C7FD-78AE-419E-B4ED-F7AD0D1FA833}" name="No. Tel Rumah Penjaga 2" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{264F72B8-EA7A-4465-87B4-33104224D9BF}" name="Jantina" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{264F72B8-EA7A-4465-87B4-33104224D9BF}" name="Jantina" dataDxfId="1">
       <calculatedColumnFormula array="1">L2L=IF(ISNUMBER(SEARCH(Table1[[#This Row],[Column1]],Table1[[#This Row],[Column1]])),"L","P")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{4B2F1A7A-B491-4D8B-97A1-ED2F1C251771}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{4B2F1A7A-B491-4D8B-97A1-ED2F1C251771}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1642,28 +1639,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A082FB5C-E072-4AAF-B83E-F40B6FD9E595}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="6.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="6.140625" style="2"/>
+    <col min="6" max="6" width="24.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="33.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="6.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1698,13 +1695,13 @@
         <v>9</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1735,13 +1732,13 @@
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1776,11 +1773,11 @@
         <v>30</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1811,11 +1808,11 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1848,11 +1845,11 @@
         <v>43</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1883,11 +1880,11 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1918,11 +1915,11 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1953,11 +1950,11 @@
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1992,11 +1989,11 @@
         <v>69</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2029,11 +2026,11 @@
         <v>76</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2064,11 +2061,11 @@
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2099,11 +2096,11 @@
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2134,11 +2131,11 @@
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2173,11 +2170,11 @@
         <v>101</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2206,11 +2203,11 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2245,11 +2242,11 @@
         <v>114</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2262,8 +2259,8 @@
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>218</v>
+      <c r="E17" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>117</v>
@@ -2280,11 +2277,11 @@
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>10</v>
@@ -2319,11 +2316,11 @@
         <v>15</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2337,7 +2334,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>125</v>
@@ -2358,11 +2355,11 @@
         <v>130</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2376,7 +2373,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>133</v>
@@ -2393,11 +2390,11 @@
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2411,7 +2408,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>139</v>
@@ -2428,11 +2425,11 @@
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2446,7 +2443,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>145</v>
@@ -2463,11 +2460,11 @@
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2481,7 +2478,7 @@
         <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>151</v>
@@ -2498,11 +2495,11 @@
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2516,7 +2513,7 @@
         <v>18</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>157</v>
@@ -2535,11 +2532,11 @@
         <v>161</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2553,7 +2550,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>164</v>
@@ -2570,11 +2567,11 @@
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2588,7 +2585,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>170</v>
@@ -2609,11 +2606,11 @@
         <v>175</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2627,7 +2624,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>178</v>
@@ -2644,11 +2641,11 @@
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2662,7 +2659,7 @@
         <v>18</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>184</v>
@@ -2683,11 +2680,11 @@
         <v>189</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2701,7 +2698,7 @@
         <v>18</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>192</v>
@@ -2718,11 +2715,11 @@
       </c>
       <c r="K29" s="7"/>
       <c r="L29" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -2736,7 +2733,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>198</v>
@@ -2753,7 +2750,7 @@
       </c>
       <c r="K30" s="16"/>
       <c r="L30" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M30" s="13"/>
     </row>
@@ -2787,11 +2784,12 @@
     <hyperlink ref="E24" r:id="rId26" xr:uid="{348289C7-E61D-4B71-8B47-35CD7CC63F18}"/>
     <hyperlink ref="E2" r:id="rId27" xr:uid="{5B9018EB-A0C4-4752-A1F9-FC20BCEFB253}"/>
     <hyperlink ref="E12" r:id="rId28" xr:uid="{05FB3F5D-32A6-4892-AA36-100A97DDDD11}"/>
+    <hyperlink ref="E17" r:id="rId29" xr:uid="{9EEFF875-D6F7-4DE4-973F-2E89C09F42C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>